<commit_message>
MGU data with new timestamp
</commit_message>
<xml_diff>
--- a/data/Web_MEM_MGU/2022_11_mem_mgu.xlsx
+++ b/data/Web_MEM_MGU/2022_11_mem_mgu.xlsx
@@ -1392,7 +1392,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2">
-        <v>1667260800</v>
+        <v>1667250000</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -1424,7 +1424,7 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3">
-        <v>1667264400</v>
+        <v>1667253600</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -1456,7 +1456,7 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4">
-        <v>1667268000</v>
+        <v>1667257200</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
@@ -1488,7 +1488,7 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5">
-        <v>1667271600</v>
+        <v>1667260800</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
@@ -1520,7 +1520,7 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6">
-        <v>1667275200</v>
+        <v>1667264400</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
@@ -1552,7 +1552,7 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7">
-        <v>1667278800</v>
+        <v>1667268000</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
@@ -1584,7 +1584,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8">
-        <v>1667282400</v>
+        <v>1667271600</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
@@ -1616,7 +1616,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9">
-        <v>1667286000</v>
+        <v>1667275200</v>
       </c>
       <c r="B9" t="s">
         <v>17</v>
@@ -1648,7 +1648,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10">
-        <v>1667289600</v>
+        <v>1667278800</v>
       </c>
       <c r="B10" t="s">
         <v>18</v>
@@ -1680,7 +1680,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11">
-        <v>1667293200</v>
+        <v>1667282400</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
@@ -1712,7 +1712,7 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12">
-        <v>1667296800</v>
+        <v>1667286000</v>
       </c>
       <c r="B12" t="s">
         <v>20</v>
@@ -1744,7 +1744,7 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13">
-        <v>1667300400</v>
+        <v>1667289600</v>
       </c>
       <c r="B13" t="s">
         <v>21</v>
@@ -1776,7 +1776,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14">
-        <v>1667304000</v>
+        <v>1667293200</v>
       </c>
       <c r="B14" t="s">
         <v>22</v>
@@ -1808,7 +1808,7 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15">
-        <v>1667307600</v>
+        <v>1667296800</v>
       </c>
       <c r="B15" t="s">
         <v>23</v>
@@ -1840,7 +1840,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16">
-        <v>1667311200</v>
+        <v>1667300400</v>
       </c>
       <c r="B16" t="s">
         <v>24</v>
@@ -1872,7 +1872,7 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17">
-        <v>1667314800</v>
+        <v>1667304000</v>
       </c>
       <c r="B17" t="s">
         <v>25</v>
@@ -1904,7 +1904,7 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18">
-        <v>1667318400</v>
+        <v>1667307600</v>
       </c>
       <c r="B18" t="s">
         <v>26</v>
@@ -1936,7 +1936,7 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19">
-        <v>1667322000</v>
+        <v>1667311200</v>
       </c>
       <c r="B19" t="s">
         <v>27</v>
@@ -1968,7 +1968,7 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20">
-        <v>1667325600</v>
+        <v>1667314800</v>
       </c>
       <c r="B20" t="s">
         <v>28</v>
@@ -2000,7 +2000,7 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21">
-        <v>1667329200</v>
+        <v>1667318400</v>
       </c>
       <c r="B21" t="s">
         <v>29</v>
@@ -2032,7 +2032,7 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22">
-        <v>1667332800</v>
+        <v>1667322000</v>
       </c>
       <c r="B22" t="s">
         <v>30</v>
@@ -2064,7 +2064,7 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23">
-        <v>1667336400</v>
+        <v>1667325600</v>
       </c>
       <c r="B23" t="s">
         <v>31</v>
@@ -2096,7 +2096,7 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24">
-        <v>1667340000</v>
+        <v>1667329200</v>
       </c>
       <c r="B24" t="s">
         <v>32</v>
@@ -2128,7 +2128,7 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25">
-        <v>1667343600</v>
+        <v>1667332800</v>
       </c>
       <c r="B25" t="s">
         <v>33</v>
@@ -2160,7 +2160,7 @@
     </row>
     <row r="26" spans="1:10">
       <c r="A26">
-        <v>1667347200</v>
+        <v>1667336400</v>
       </c>
       <c r="B26" t="s">
         <v>34</v>
@@ -2192,7 +2192,7 @@
     </row>
     <row r="27" spans="1:10">
       <c r="A27">
-        <v>1667350800</v>
+        <v>1667340000</v>
       </c>
       <c r="B27" t="s">
         <v>35</v>
@@ -2224,7 +2224,7 @@
     </row>
     <row r="28" spans="1:10">
       <c r="A28">
-        <v>1667354400</v>
+        <v>1667343600</v>
       </c>
       <c r="B28" t="s">
         <v>36</v>
@@ -2256,7 +2256,7 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29">
-        <v>1667358000</v>
+        <v>1667347200</v>
       </c>
       <c r="B29" t="s">
         <v>37</v>
@@ -2288,7 +2288,7 @@
     </row>
     <row r="30" spans="1:10">
       <c r="A30">
-        <v>1667361600</v>
+        <v>1667350800</v>
       </c>
       <c r="B30" t="s">
         <v>38</v>
@@ -2320,7 +2320,7 @@
     </row>
     <row r="31" spans="1:10">
       <c r="A31">
-        <v>1667365200</v>
+        <v>1667354400</v>
       </c>
       <c r="B31" t="s">
         <v>39</v>
@@ -2352,7 +2352,7 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32">
-        <v>1667368800</v>
+        <v>1667358000</v>
       </c>
       <c r="B32" t="s">
         <v>40</v>
@@ -2384,7 +2384,7 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33">
-        <v>1667372400</v>
+        <v>1667361600</v>
       </c>
       <c r="B33" t="s">
         <v>41</v>
@@ -2416,7 +2416,7 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34">
-        <v>1667376000</v>
+        <v>1667365200</v>
       </c>
       <c r="B34" t="s">
         <v>42</v>
@@ -2448,7 +2448,7 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35">
-        <v>1667379600</v>
+        <v>1667368800</v>
       </c>
       <c r="B35" t="s">
         <v>43</v>
@@ -2480,7 +2480,7 @@
     </row>
     <row r="36" spans="1:10">
       <c r="A36">
-        <v>1667383200</v>
+        <v>1667372400</v>
       </c>
       <c r="B36" t="s">
         <v>44</v>
@@ -2512,7 +2512,7 @@
     </row>
     <row r="37" spans="1:10">
       <c r="A37">
-        <v>1667386800</v>
+        <v>1667376000</v>
       </c>
       <c r="B37" t="s">
         <v>45</v>
@@ -2544,7 +2544,7 @@
     </row>
     <row r="38" spans="1:10">
       <c r="A38">
-        <v>1667390400</v>
+        <v>1667379600</v>
       </c>
       <c r="B38" t="s">
         <v>46</v>
@@ -2576,7 +2576,7 @@
     </row>
     <row r="39" spans="1:10">
       <c r="A39">
-        <v>1667394000</v>
+        <v>1667383200</v>
       </c>
       <c r="B39" t="s">
         <v>47</v>
@@ -2608,7 +2608,7 @@
     </row>
     <row r="40" spans="1:10">
       <c r="A40">
-        <v>1667397600</v>
+        <v>1667386800</v>
       </c>
       <c r="B40" t="s">
         <v>48</v>
@@ -2640,7 +2640,7 @@
     </row>
     <row r="41" spans="1:10">
       <c r="A41">
-        <v>1667401200</v>
+        <v>1667390400</v>
       </c>
       <c r="B41" t="s">
         <v>49</v>
@@ -2672,7 +2672,7 @@
     </row>
     <row r="42" spans="1:10">
       <c r="A42">
-        <v>1667404800</v>
+        <v>1667394000</v>
       </c>
       <c r="B42" t="s">
         <v>50</v>
@@ -2704,7 +2704,7 @@
     </row>
     <row r="43" spans="1:10">
       <c r="A43">
-        <v>1667408400</v>
+        <v>1667397600</v>
       </c>
       <c r="B43" t="s">
         <v>51</v>
@@ -2736,7 +2736,7 @@
     </row>
     <row r="44" spans="1:10">
       <c r="A44">
-        <v>1667412000</v>
+        <v>1667401200</v>
       </c>
       <c r="B44" t="s">
         <v>52</v>
@@ -2768,7 +2768,7 @@
     </row>
     <row r="45" spans="1:10">
       <c r="A45">
-        <v>1667415600</v>
+        <v>1667404800</v>
       </c>
       <c r="B45" t="s">
         <v>53</v>
@@ -2800,7 +2800,7 @@
     </row>
     <row r="46" spans="1:10">
       <c r="A46">
-        <v>1667419200</v>
+        <v>1667408400</v>
       </c>
       <c r="B46" t="s">
         <v>54</v>
@@ -2832,7 +2832,7 @@
     </row>
     <row r="47" spans="1:10">
       <c r="A47">
-        <v>1667422800</v>
+        <v>1667412000</v>
       </c>
       <c r="B47" t="s">
         <v>55</v>
@@ -2864,7 +2864,7 @@
     </row>
     <row r="48" spans="1:10">
       <c r="A48">
-        <v>1667426400</v>
+        <v>1667415600</v>
       </c>
       <c r="B48" t="s">
         <v>56</v>
@@ -2896,7 +2896,7 @@
     </row>
     <row r="49" spans="1:10">
       <c r="A49">
-        <v>1667430000</v>
+        <v>1667419200</v>
       </c>
       <c r="B49" t="s">
         <v>57</v>
@@ -2928,7 +2928,7 @@
     </row>
     <row r="50" spans="1:10">
       <c r="A50">
-        <v>1667433600</v>
+        <v>1667422800</v>
       </c>
       <c r="B50" t="s">
         <v>58</v>
@@ -2960,7 +2960,7 @@
     </row>
     <row r="51" spans="1:10">
       <c r="A51">
-        <v>1667437200</v>
+        <v>1667426400</v>
       </c>
       <c r="B51" t="s">
         <v>59</v>
@@ -2992,7 +2992,7 @@
     </row>
     <row r="52" spans="1:10">
       <c r="A52">
-        <v>1667440800</v>
+        <v>1667430000</v>
       </c>
       <c r="B52" t="s">
         <v>60</v>
@@ -3024,7 +3024,7 @@
     </row>
     <row r="53" spans="1:10">
       <c r="A53">
-        <v>1667444400</v>
+        <v>1667433600</v>
       </c>
       <c r="B53" t="s">
         <v>61</v>
@@ -3056,7 +3056,7 @@
     </row>
     <row r="54" spans="1:10">
       <c r="A54">
-        <v>1667448000</v>
+        <v>1667437200</v>
       </c>
       <c r="B54" t="s">
         <v>62</v>
@@ -3088,7 +3088,7 @@
     </row>
     <row r="55" spans="1:10">
       <c r="A55">
-        <v>1667451600</v>
+        <v>1667440800</v>
       </c>
       <c r="B55" t="s">
         <v>63</v>
@@ -3120,7 +3120,7 @@
     </row>
     <row r="56" spans="1:10">
       <c r="A56">
-        <v>1667455200</v>
+        <v>1667444400</v>
       </c>
       <c r="B56" t="s">
         <v>64</v>
@@ -3152,7 +3152,7 @@
     </row>
     <row r="57" spans="1:10">
       <c r="A57">
-        <v>1667458800</v>
+        <v>1667448000</v>
       </c>
       <c r="B57" t="s">
         <v>65</v>
@@ -3184,7 +3184,7 @@
     </row>
     <row r="58" spans="1:10">
       <c r="A58">
-        <v>1667462400</v>
+        <v>1667451600</v>
       </c>
       <c r="B58" t="s">
         <v>66</v>
@@ -3216,7 +3216,7 @@
     </row>
     <row r="59" spans="1:10">
       <c r="A59">
-        <v>1667466000</v>
+        <v>1667455200</v>
       </c>
       <c r="B59" t="s">
         <v>67</v>
@@ -3248,7 +3248,7 @@
     </row>
     <row r="60" spans="1:10">
       <c r="A60">
-        <v>1667469600</v>
+        <v>1667458800</v>
       </c>
       <c r="B60" t="s">
         <v>68</v>
@@ -3280,7 +3280,7 @@
     </row>
     <row r="61" spans="1:10">
       <c r="A61">
-        <v>1667473200</v>
+        <v>1667462400</v>
       </c>
       <c r="B61" t="s">
         <v>69</v>
@@ -3312,7 +3312,7 @@
     </row>
     <row r="62" spans="1:10">
       <c r="A62">
-        <v>1667476800</v>
+        <v>1667466000</v>
       </c>
       <c r="B62" t="s">
         <v>70</v>
@@ -3344,7 +3344,7 @@
     </row>
     <row r="63" spans="1:10">
       <c r="A63">
-        <v>1667480400</v>
+        <v>1667469600</v>
       </c>
       <c r="B63" t="s">
         <v>71</v>
@@ -3376,7 +3376,7 @@
     </row>
     <row r="64" spans="1:10">
       <c r="A64">
-        <v>1667484000</v>
+        <v>1667473200</v>
       </c>
       <c r="B64" t="s">
         <v>72</v>
@@ -3408,7 +3408,7 @@
     </row>
     <row r="65" spans="1:10">
       <c r="A65">
-        <v>1667487600</v>
+        <v>1667476800</v>
       </c>
       <c r="B65" t="s">
         <v>73</v>
@@ -3440,7 +3440,7 @@
     </row>
     <row r="66" spans="1:10">
       <c r="A66">
-        <v>1667491200</v>
+        <v>1667480400</v>
       </c>
       <c r="B66" t="s">
         <v>74</v>
@@ -3472,7 +3472,7 @@
     </row>
     <row r="67" spans="1:10">
       <c r="A67">
-        <v>1667494800</v>
+        <v>1667484000</v>
       </c>
       <c r="B67" t="s">
         <v>75</v>
@@ -3504,7 +3504,7 @@
     </row>
     <row r="68" spans="1:10">
       <c r="A68">
-        <v>1667498400</v>
+        <v>1667487600</v>
       </c>
       <c r="B68" t="s">
         <v>76</v>
@@ -3536,7 +3536,7 @@
     </row>
     <row r="69" spans="1:10">
       <c r="A69">
-        <v>1667502000</v>
+        <v>1667491200</v>
       </c>
       <c r="B69" t="s">
         <v>77</v>
@@ -3568,7 +3568,7 @@
     </row>
     <row r="70" spans="1:10">
       <c r="A70">
-        <v>1667505600</v>
+        <v>1667494800</v>
       </c>
       <c r="B70" t="s">
         <v>78</v>
@@ -3600,7 +3600,7 @@
     </row>
     <row r="71" spans="1:10">
       <c r="A71">
-        <v>1667509200</v>
+        <v>1667498400</v>
       </c>
       <c r="B71" t="s">
         <v>79</v>
@@ -3632,7 +3632,7 @@
     </row>
     <row r="72" spans="1:10">
       <c r="A72">
-        <v>1667512800</v>
+        <v>1667502000</v>
       </c>
       <c r="B72" t="s">
         <v>80</v>
@@ -3664,7 +3664,7 @@
     </row>
     <row r="73" spans="1:10">
       <c r="A73">
-        <v>1667516400</v>
+        <v>1667505600</v>
       </c>
       <c r="B73" t="s">
         <v>81</v>
@@ -3696,7 +3696,7 @@
     </row>
     <row r="74" spans="1:10">
       <c r="A74">
-        <v>1667520000</v>
+        <v>1667509200</v>
       </c>
       <c r="B74" t="s">
         <v>82</v>
@@ -3728,7 +3728,7 @@
     </row>
     <row r="75" spans="1:10">
       <c r="A75">
-        <v>1667523600</v>
+        <v>1667512800</v>
       </c>
       <c r="B75" t="s">
         <v>83</v>
@@ -3760,7 +3760,7 @@
     </row>
     <row r="76" spans="1:10">
       <c r="A76">
-        <v>1667527200</v>
+        <v>1667516400</v>
       </c>
       <c r="B76" t="s">
         <v>84</v>
@@ -3792,7 +3792,7 @@
     </row>
     <row r="77" spans="1:10">
       <c r="A77">
-        <v>1667530800</v>
+        <v>1667520000</v>
       </c>
       <c r="B77" t="s">
         <v>85</v>
@@ -3824,7 +3824,7 @@
     </row>
     <row r="78" spans="1:10">
       <c r="A78">
-        <v>1667534400</v>
+        <v>1667523600</v>
       </c>
       <c r="B78" t="s">
         <v>86</v>
@@ -3856,7 +3856,7 @@
     </row>
     <row r="79" spans="1:10">
       <c r="A79">
-        <v>1667538000</v>
+        <v>1667527200</v>
       </c>
       <c r="B79" t="s">
         <v>87</v>
@@ -3888,7 +3888,7 @@
     </row>
     <row r="80" spans="1:10">
       <c r="A80">
-        <v>1667541600</v>
+        <v>1667530800</v>
       </c>
       <c r="B80" t="s">
         <v>88</v>
@@ -3920,7 +3920,7 @@
     </row>
     <row r="81" spans="1:10">
       <c r="A81">
-        <v>1667545200</v>
+        <v>1667534400</v>
       </c>
       <c r="B81" t="s">
         <v>89</v>
@@ -3952,7 +3952,7 @@
     </row>
     <row r="82" spans="1:10">
       <c r="A82">
-        <v>1667548800</v>
+        <v>1667538000</v>
       </c>
       <c r="B82" t="s">
         <v>90</v>
@@ -3984,7 +3984,7 @@
     </row>
     <row r="83" spans="1:10">
       <c r="A83">
-        <v>1667552400</v>
+        <v>1667541600</v>
       </c>
       <c r="B83" t="s">
         <v>91</v>
@@ -4016,7 +4016,7 @@
     </row>
     <row r="84" spans="1:10">
       <c r="A84">
-        <v>1667556000</v>
+        <v>1667545200</v>
       </c>
       <c r="B84" t="s">
         <v>92</v>
@@ -4048,7 +4048,7 @@
     </row>
     <row r="85" spans="1:10">
       <c r="A85">
-        <v>1667559600</v>
+        <v>1667548800</v>
       </c>
       <c r="B85" t="s">
         <v>93</v>
@@ -4080,7 +4080,7 @@
     </row>
     <row r="86" spans="1:10">
       <c r="A86">
-        <v>1667563200</v>
+        <v>1667552400</v>
       </c>
       <c r="B86" t="s">
         <v>94</v>
@@ -4112,7 +4112,7 @@
     </row>
     <row r="87" spans="1:10">
       <c r="A87">
-        <v>1667566800</v>
+        <v>1667556000</v>
       </c>
       <c r="B87" t="s">
         <v>95</v>
@@ -4144,7 +4144,7 @@
     </row>
     <row r="88" spans="1:10">
       <c r="A88">
-        <v>1667570400</v>
+        <v>1667559600</v>
       </c>
       <c r="B88" t="s">
         <v>96</v>
@@ -4176,7 +4176,7 @@
     </row>
     <row r="89" spans="1:10">
       <c r="A89">
-        <v>1667574000</v>
+        <v>1667563200</v>
       </c>
       <c r="B89" t="s">
         <v>97</v>
@@ -4208,7 +4208,7 @@
     </row>
     <row r="90" spans="1:10">
       <c r="A90">
-        <v>1667577600</v>
+        <v>1667566800</v>
       </c>
       <c r="B90" t="s">
         <v>98</v>
@@ -4240,7 +4240,7 @@
     </row>
     <row r="91" spans="1:10">
       <c r="A91">
-        <v>1667581200</v>
+        <v>1667570400</v>
       </c>
       <c r="B91" t="s">
         <v>99</v>
@@ -4272,7 +4272,7 @@
     </row>
     <row r="92" spans="1:10">
       <c r="A92">
-        <v>1667584800</v>
+        <v>1667574000</v>
       </c>
       <c r="B92" t="s">
         <v>100</v>
@@ -4304,7 +4304,7 @@
     </row>
     <row r="93" spans="1:10">
       <c r="A93">
-        <v>1667588400</v>
+        <v>1667577600</v>
       </c>
       <c r="B93" t="s">
         <v>101</v>
@@ -4336,7 +4336,7 @@
     </row>
     <row r="94" spans="1:10">
       <c r="A94">
-        <v>1667592000</v>
+        <v>1667581200</v>
       </c>
       <c r="B94" t="s">
         <v>102</v>
@@ -4368,7 +4368,7 @@
     </row>
     <row r="95" spans="1:10">
       <c r="A95">
-        <v>1667595600</v>
+        <v>1667584800</v>
       </c>
       <c r="B95" t="s">
         <v>103</v>
@@ -4400,7 +4400,7 @@
     </row>
     <row r="96" spans="1:10">
       <c r="A96">
-        <v>1667599200</v>
+        <v>1667588400</v>
       </c>
       <c r="B96" t="s">
         <v>104</v>
@@ -4432,7 +4432,7 @@
     </row>
     <row r="97" spans="1:10">
       <c r="A97">
-        <v>1667602800</v>
+        <v>1667592000</v>
       </c>
       <c r="B97" t="s">
         <v>105</v>
@@ -4464,7 +4464,7 @@
     </row>
     <row r="98" spans="1:10">
       <c r="A98">
-        <v>1667606400</v>
+        <v>1667595600</v>
       </c>
       <c r="B98" t="s">
         <v>106</v>
@@ -4496,7 +4496,7 @@
     </row>
     <row r="99" spans="1:10">
       <c r="A99">
-        <v>1667610000</v>
+        <v>1667599200</v>
       </c>
       <c r="B99" t="s">
         <v>107</v>
@@ -4528,7 +4528,7 @@
     </row>
     <row r="100" spans="1:10">
       <c r="A100">
-        <v>1667613600</v>
+        <v>1667602800</v>
       </c>
       <c r="B100" t="s">
         <v>108</v>
@@ -4560,7 +4560,7 @@
     </row>
     <row r="101" spans="1:10">
       <c r="A101">
-        <v>1667617200</v>
+        <v>1667606400</v>
       </c>
       <c r="B101" t="s">
         <v>109</v>
@@ -4592,7 +4592,7 @@
     </row>
     <row r="102" spans="1:10">
       <c r="A102">
-        <v>1667620800</v>
+        <v>1667610000</v>
       </c>
       <c r="B102" t="s">
         <v>110</v>
@@ -4624,7 +4624,7 @@
     </row>
     <row r="103" spans="1:10">
       <c r="A103">
-        <v>1667624400</v>
+        <v>1667613600</v>
       </c>
       <c r="B103" t="s">
         <v>111</v>
@@ -4656,7 +4656,7 @@
     </row>
     <row r="104" spans="1:10">
       <c r="A104">
-        <v>1667628000</v>
+        <v>1667617200</v>
       </c>
       <c r="B104" t="s">
         <v>112</v>
@@ -4688,7 +4688,7 @@
     </row>
     <row r="105" spans="1:10">
       <c r="A105">
-        <v>1667631600</v>
+        <v>1667620800</v>
       </c>
       <c r="B105" t="s">
         <v>113</v>
@@ -4720,7 +4720,7 @@
     </row>
     <row r="106" spans="1:10">
       <c r="A106">
-        <v>1667635200</v>
+        <v>1667624400</v>
       </c>
       <c r="B106" t="s">
         <v>114</v>
@@ -4752,7 +4752,7 @@
     </row>
     <row r="107" spans="1:10">
       <c r="A107">
-        <v>1667638800</v>
+        <v>1667628000</v>
       </c>
       <c r="B107" t="s">
         <v>115</v>
@@ -4784,7 +4784,7 @@
     </row>
     <row r="108" spans="1:10">
       <c r="A108">
-        <v>1667642400</v>
+        <v>1667631600</v>
       </c>
       <c r="B108" t="s">
         <v>116</v>
@@ -4816,7 +4816,7 @@
     </row>
     <row r="109" spans="1:10">
       <c r="A109">
-        <v>1667646000</v>
+        <v>1667635200</v>
       </c>
       <c r="B109" t="s">
         <v>117</v>
@@ -4848,7 +4848,7 @@
     </row>
     <row r="110" spans="1:10">
       <c r="A110">
-        <v>1667649600</v>
+        <v>1667638800</v>
       </c>
       <c r="B110" t="s">
         <v>118</v>
@@ -4880,7 +4880,7 @@
     </row>
     <row r="111" spans="1:10">
       <c r="A111">
-        <v>1667653200</v>
+        <v>1667642400</v>
       </c>
       <c r="B111" t="s">
         <v>119</v>
@@ -4912,7 +4912,7 @@
     </row>
     <row r="112" spans="1:10">
       <c r="A112">
-        <v>1667656800</v>
+        <v>1667646000</v>
       </c>
       <c r="B112" t="s">
         <v>120</v>
@@ -4944,7 +4944,7 @@
     </row>
     <row r="113" spans="1:10">
       <c r="A113">
-        <v>1667660400</v>
+        <v>1667649600</v>
       </c>
       <c r="B113" t="s">
         <v>121</v>
@@ -4976,7 +4976,7 @@
     </row>
     <row r="114" spans="1:10">
       <c r="A114">
-        <v>1667664000</v>
+        <v>1667653200</v>
       </c>
       <c r="B114" t="s">
         <v>122</v>
@@ -5008,7 +5008,7 @@
     </row>
     <row r="115" spans="1:10">
       <c r="A115">
-        <v>1667667600</v>
+        <v>1667656800</v>
       </c>
       <c r="B115" t="s">
         <v>123</v>
@@ -5040,7 +5040,7 @@
     </row>
     <row r="116" spans="1:10">
       <c r="A116">
-        <v>1667671200</v>
+        <v>1667660400</v>
       </c>
       <c r="B116" t="s">
         <v>124</v>
@@ -5072,7 +5072,7 @@
     </row>
     <row r="117" spans="1:10">
       <c r="A117">
-        <v>1667674800</v>
+        <v>1667664000</v>
       </c>
       <c r="B117" t="s">
         <v>125</v>
@@ -5104,7 +5104,7 @@
     </row>
     <row r="118" spans="1:10">
       <c r="A118">
-        <v>1667678400</v>
+        <v>1667667600</v>
       </c>
       <c r="B118" t="s">
         <v>126</v>
@@ -5136,7 +5136,7 @@
     </row>
     <row r="119" spans="1:10">
       <c r="A119">
-        <v>1667682000</v>
+        <v>1667671200</v>
       </c>
       <c r="B119" t="s">
         <v>127</v>
@@ -5168,7 +5168,7 @@
     </row>
     <row r="120" spans="1:10">
       <c r="A120">
-        <v>1667685600</v>
+        <v>1667674800</v>
       </c>
       <c r="B120" t="s">
         <v>128</v>
@@ -5200,7 +5200,7 @@
     </row>
     <row r="121" spans="1:10">
       <c r="A121">
-        <v>1667689200</v>
+        <v>1667678400</v>
       </c>
       <c r="B121" t="s">
         <v>129</v>
@@ -5232,7 +5232,7 @@
     </row>
     <row r="122" spans="1:10">
       <c r="A122">
-        <v>1667692800</v>
+        <v>1667682000</v>
       </c>
       <c r="B122" t="s">
         <v>130</v>
@@ -5264,7 +5264,7 @@
     </row>
     <row r="123" spans="1:10">
       <c r="A123">
-        <v>1667696400</v>
+        <v>1667685600</v>
       </c>
       <c r="B123" t="s">
         <v>131</v>
@@ -5296,7 +5296,7 @@
     </row>
     <row r="124" spans="1:10">
       <c r="A124">
-        <v>1667700000</v>
+        <v>1667689200</v>
       </c>
       <c r="B124" t="s">
         <v>132</v>
@@ -5328,7 +5328,7 @@
     </row>
     <row r="125" spans="1:10">
       <c r="A125">
-        <v>1667703600</v>
+        <v>1667692800</v>
       </c>
       <c r="B125" t="s">
         <v>133</v>
@@ -5360,7 +5360,7 @@
     </row>
     <row r="126" spans="1:10">
       <c r="A126">
-        <v>1667707200</v>
+        <v>1667696400</v>
       </c>
       <c r="B126" t="s">
         <v>134</v>
@@ -5392,7 +5392,7 @@
     </row>
     <row r="127" spans="1:10">
       <c r="A127">
-        <v>1667710800</v>
+        <v>1667700000</v>
       </c>
       <c r="B127" t="s">
         <v>135</v>
@@ -5424,7 +5424,7 @@
     </row>
     <row r="128" spans="1:10">
       <c r="A128">
-        <v>1667714400</v>
+        <v>1667703600</v>
       </c>
       <c r="B128" t="s">
         <v>136</v>
@@ -5456,7 +5456,7 @@
     </row>
     <row r="129" spans="1:10">
       <c r="A129">
-        <v>1667718000</v>
+        <v>1667707200</v>
       </c>
       <c r="B129" t="s">
         <v>137</v>
@@ -5488,7 +5488,7 @@
     </row>
     <row r="130" spans="1:10">
       <c r="A130">
-        <v>1667721600</v>
+        <v>1667710800</v>
       </c>
       <c r="B130" t="s">
         <v>138</v>
@@ -5520,7 +5520,7 @@
     </row>
     <row r="131" spans="1:10">
       <c r="A131">
-        <v>1667725200</v>
+        <v>1667714400</v>
       </c>
       <c r="B131" t="s">
         <v>139</v>
@@ -5552,7 +5552,7 @@
     </row>
     <row r="132" spans="1:10">
       <c r="A132">
-        <v>1667728800</v>
+        <v>1667718000</v>
       </c>
       <c r="B132" t="s">
         <v>140</v>
@@ -5584,7 +5584,7 @@
     </row>
     <row r="133" spans="1:10">
       <c r="A133">
-        <v>1667732400</v>
+        <v>1667721600</v>
       </c>
       <c r="B133" t="s">
         <v>141</v>
@@ -5616,7 +5616,7 @@
     </row>
     <row r="134" spans="1:10">
       <c r="A134">
-        <v>1667736000</v>
+        <v>1667725200</v>
       </c>
       <c r="B134" t="s">
         <v>142</v>
@@ -5648,7 +5648,7 @@
     </row>
     <row r="135" spans="1:10">
       <c r="A135">
-        <v>1667739600</v>
+        <v>1667728800</v>
       </c>
       <c r="B135" t="s">
         <v>143</v>
@@ -5680,7 +5680,7 @@
     </row>
     <row r="136" spans="1:10">
       <c r="A136">
-        <v>1667743200</v>
+        <v>1667732400</v>
       </c>
       <c r="B136" t="s">
         <v>144</v>
@@ -5712,7 +5712,7 @@
     </row>
     <row r="137" spans="1:10">
       <c r="A137">
-        <v>1667746800</v>
+        <v>1667736000</v>
       </c>
       <c r="B137" t="s">
         <v>145</v>
@@ -5744,7 +5744,7 @@
     </row>
     <row r="138" spans="1:10">
       <c r="A138">
-        <v>1667750400</v>
+        <v>1667739600</v>
       </c>
       <c r="B138" t="s">
         <v>146</v>
@@ -5776,7 +5776,7 @@
     </row>
     <row r="139" spans="1:10">
       <c r="A139">
-        <v>1667754000</v>
+        <v>1667743200</v>
       </c>
       <c r="B139" t="s">
         <v>147</v>
@@ -5808,7 +5808,7 @@
     </row>
     <row r="140" spans="1:10">
       <c r="A140">
-        <v>1667757600</v>
+        <v>1667746800</v>
       </c>
       <c r="B140" t="s">
         <v>148</v>
@@ -5840,7 +5840,7 @@
     </row>
     <row r="141" spans="1:10">
       <c r="A141">
-        <v>1667761200</v>
+        <v>1667750400</v>
       </c>
       <c r="B141" t="s">
         <v>149</v>
@@ -5872,7 +5872,7 @@
     </row>
     <row r="142" spans="1:10">
       <c r="A142">
-        <v>1667764800</v>
+        <v>1667754000</v>
       </c>
       <c r="B142" t="s">
         <v>150</v>
@@ -5904,7 +5904,7 @@
     </row>
     <row r="143" spans="1:10">
       <c r="A143">
-        <v>1667768400</v>
+        <v>1667757600</v>
       </c>
       <c r="B143" t="s">
         <v>151</v>
@@ -5936,7 +5936,7 @@
     </row>
     <row r="144" spans="1:10">
       <c r="A144">
-        <v>1667772000</v>
+        <v>1667761200</v>
       </c>
       <c r="B144" t="s">
         <v>152</v>
@@ -5968,7 +5968,7 @@
     </row>
     <row r="145" spans="1:10">
       <c r="A145">
-        <v>1667775600</v>
+        <v>1667764800</v>
       </c>
       <c r="B145" t="s">
         <v>153</v>
@@ -6000,7 +6000,7 @@
     </row>
     <row r="146" spans="1:10">
       <c r="A146">
-        <v>1667779200</v>
+        <v>1667768400</v>
       </c>
       <c r="B146" t="s">
         <v>154</v>
@@ -6032,7 +6032,7 @@
     </row>
     <row r="147" spans="1:10">
       <c r="A147">
-        <v>1667782800</v>
+        <v>1667772000</v>
       </c>
       <c r="B147" t="s">
         <v>155</v>
@@ -6064,7 +6064,7 @@
     </row>
     <row r="148" spans="1:10">
       <c r="A148">
-        <v>1667786400</v>
+        <v>1667775600</v>
       </c>
       <c r="B148" t="s">
         <v>156</v>
@@ -6096,7 +6096,7 @@
     </row>
     <row r="149" spans="1:10">
       <c r="A149">
-        <v>1667790000</v>
+        <v>1667779200</v>
       </c>
       <c r="B149" t="s">
         <v>157</v>
@@ -6128,7 +6128,7 @@
     </row>
     <row r="150" spans="1:10">
       <c r="A150">
-        <v>1667793600</v>
+        <v>1667782800</v>
       </c>
       <c r="B150" t="s">
         <v>158</v>
@@ -6160,7 +6160,7 @@
     </row>
     <row r="151" spans="1:10">
       <c r="A151">
-        <v>1667797200</v>
+        <v>1667786400</v>
       </c>
       <c r="B151" t="s">
         <v>159</v>
@@ -6192,7 +6192,7 @@
     </row>
     <row r="152" spans="1:10">
       <c r="A152">
-        <v>1667800800</v>
+        <v>1667790000</v>
       </c>
       <c r="B152" t="s">
         <v>160</v>
@@ -6224,7 +6224,7 @@
     </row>
     <row r="153" spans="1:10">
       <c r="A153">
-        <v>1667804400</v>
+        <v>1667793600</v>
       </c>
       <c r="B153" t="s">
         <v>161</v>
@@ -6256,7 +6256,7 @@
     </row>
     <row r="154" spans="1:10">
       <c r="A154">
-        <v>1667808000</v>
+        <v>1667797200</v>
       </c>
       <c r="B154" t="s">
         <v>162</v>
@@ -6288,7 +6288,7 @@
     </row>
     <row r="155" spans="1:10">
       <c r="A155">
-        <v>1667811600</v>
+        <v>1667800800</v>
       </c>
       <c r="B155" t="s">
         <v>163</v>
@@ -6320,7 +6320,7 @@
     </row>
     <row r="156" spans="1:10">
       <c r="A156">
-        <v>1667815200</v>
+        <v>1667804400</v>
       </c>
       <c r="B156" t="s">
         <v>164</v>
@@ -6352,7 +6352,7 @@
     </row>
     <row r="157" spans="1:10">
       <c r="A157">
-        <v>1667818800</v>
+        <v>1667808000</v>
       </c>
       <c r="B157" t="s">
         <v>165</v>
@@ -6384,7 +6384,7 @@
     </row>
     <row r="158" spans="1:10">
       <c r="A158">
-        <v>1667822400</v>
+        <v>1667811600</v>
       </c>
       <c r="B158" t="s">
         <v>166</v>
@@ -6416,7 +6416,7 @@
     </row>
     <row r="159" spans="1:10">
       <c r="A159">
-        <v>1667826000</v>
+        <v>1667815200</v>
       </c>
       <c r="B159" t="s">
         <v>167</v>
@@ -6448,7 +6448,7 @@
     </row>
     <row r="160" spans="1:10">
       <c r="A160">
-        <v>1667829600</v>
+        <v>1667818800</v>
       </c>
       <c r="B160" t="s">
         <v>168</v>
@@ -6480,7 +6480,7 @@
     </row>
     <row r="161" spans="1:10">
       <c r="A161">
-        <v>1667833200</v>
+        <v>1667822400</v>
       </c>
       <c r="B161" t="s">
         <v>169</v>
@@ -6512,7 +6512,7 @@
     </row>
     <row r="162" spans="1:10">
       <c r="A162">
-        <v>1667836800</v>
+        <v>1667826000</v>
       </c>
       <c r="B162" t="s">
         <v>170</v>
@@ -6544,7 +6544,7 @@
     </row>
     <row r="163" spans="1:10">
       <c r="A163">
-        <v>1667840400</v>
+        <v>1667829600</v>
       </c>
       <c r="B163" t="s">
         <v>171</v>
@@ -6576,7 +6576,7 @@
     </row>
     <row r="164" spans="1:10">
       <c r="A164">
-        <v>1667844000</v>
+        <v>1667833200</v>
       </c>
       <c r="B164" t="s">
         <v>172</v>
@@ -6608,7 +6608,7 @@
     </row>
     <row r="165" spans="1:10">
       <c r="A165">
-        <v>1667847600</v>
+        <v>1667836800</v>
       </c>
       <c r="B165" t="s">
         <v>173</v>
@@ -6640,7 +6640,7 @@
     </row>
     <row r="166" spans="1:10">
       <c r="A166">
-        <v>1667851200</v>
+        <v>1667840400</v>
       </c>
       <c r="B166" t="s">
         <v>174</v>
@@ -6672,7 +6672,7 @@
     </row>
     <row r="167" spans="1:10">
       <c r="A167">
-        <v>1667854800</v>
+        <v>1667844000</v>
       </c>
       <c r="B167" t="s">
         <v>175</v>
@@ -6704,7 +6704,7 @@
     </row>
     <row r="168" spans="1:10">
       <c r="A168">
-        <v>1667858400</v>
+        <v>1667847600</v>
       </c>
       <c r="B168" t="s">
         <v>176</v>
@@ -6736,7 +6736,7 @@
     </row>
     <row r="169" spans="1:10">
       <c r="A169">
-        <v>1667862000</v>
+        <v>1667851200</v>
       </c>
       <c r="B169" t="s">
         <v>177</v>
@@ -6768,7 +6768,7 @@
     </row>
     <row r="170" spans="1:10">
       <c r="A170">
-        <v>1667865600</v>
+        <v>1667854800</v>
       </c>
       <c r="B170" t="s">
         <v>178</v>
@@ -6800,7 +6800,7 @@
     </row>
     <row r="171" spans="1:10">
       <c r="A171">
-        <v>1667869200</v>
+        <v>1667858400</v>
       </c>
       <c r="B171" t="s">
         <v>179</v>
@@ -6832,7 +6832,7 @@
     </row>
     <row r="172" spans="1:10">
       <c r="A172">
-        <v>1667872800</v>
+        <v>1667862000</v>
       </c>
       <c r="B172" t="s">
         <v>180</v>
@@ -6864,7 +6864,7 @@
     </row>
     <row r="173" spans="1:10">
       <c r="A173">
-        <v>1667876400</v>
+        <v>1667865600</v>
       </c>
       <c r="B173" t="s">
         <v>181</v>
@@ -6896,7 +6896,7 @@
     </row>
     <row r="174" spans="1:10">
       <c r="A174">
-        <v>1667880000</v>
+        <v>1667869200</v>
       </c>
       <c r="B174" t="s">
         <v>182</v>
@@ -6928,7 +6928,7 @@
     </row>
     <row r="175" spans="1:10">
       <c r="A175">
-        <v>1667883600</v>
+        <v>1667872800</v>
       </c>
       <c r="B175" t="s">
         <v>183</v>
@@ -6960,7 +6960,7 @@
     </row>
     <row r="176" spans="1:10">
       <c r="A176">
-        <v>1667887200</v>
+        <v>1667876400</v>
       </c>
       <c r="B176" t="s">
         <v>184</v>
@@ -6992,7 +6992,7 @@
     </row>
     <row r="177" spans="1:10">
       <c r="A177">
-        <v>1667890800</v>
+        <v>1667880000</v>
       </c>
       <c r="B177" t="s">
         <v>185</v>
@@ -7024,7 +7024,7 @@
     </row>
     <row r="178" spans="1:10">
       <c r="A178">
-        <v>1667894400</v>
+        <v>1667883600</v>
       </c>
       <c r="B178" t="s">
         <v>186</v>
@@ -7056,7 +7056,7 @@
     </row>
     <row r="179" spans="1:10">
       <c r="A179">
-        <v>1667898000</v>
+        <v>1667887200</v>
       </c>
       <c r="B179" t="s">
         <v>187</v>
@@ -7088,7 +7088,7 @@
     </row>
     <row r="180" spans="1:10">
       <c r="A180">
-        <v>1667901600</v>
+        <v>1667890800</v>
       </c>
       <c r="B180" t="s">
         <v>188</v>
@@ -7120,7 +7120,7 @@
     </row>
     <row r="181" spans="1:10">
       <c r="A181">
-        <v>1667905200</v>
+        <v>1667894400</v>
       </c>
       <c r="B181" t="s">
         <v>189</v>
@@ -7152,7 +7152,7 @@
     </row>
     <row r="182" spans="1:10">
       <c r="A182">
-        <v>1667908800</v>
+        <v>1667898000</v>
       </c>
       <c r="B182" t="s">
         <v>190</v>
@@ -7184,7 +7184,7 @@
     </row>
     <row r="183" spans="1:10">
       <c r="A183">
-        <v>1667912400</v>
+        <v>1667901600</v>
       </c>
       <c r="B183" t="s">
         <v>191</v>
@@ -7216,7 +7216,7 @@
     </row>
     <row r="184" spans="1:10">
       <c r="A184">
-        <v>1667916000</v>
+        <v>1667905200</v>
       </c>
       <c r="B184" t="s">
         <v>192</v>
@@ -7248,7 +7248,7 @@
     </row>
     <row r="185" spans="1:10">
       <c r="A185">
-        <v>1667919600</v>
+        <v>1667908800</v>
       </c>
       <c r="B185" t="s">
         <v>193</v>
@@ -7280,7 +7280,7 @@
     </row>
     <row r="186" spans="1:10">
       <c r="A186">
-        <v>1667923200</v>
+        <v>1667912400</v>
       </c>
       <c r="B186" t="s">
         <v>194</v>
@@ -7312,7 +7312,7 @@
     </row>
     <row r="187" spans="1:10">
       <c r="A187">
-        <v>1667926800</v>
+        <v>1667916000</v>
       </c>
       <c r="B187" t="s">
         <v>195</v>
@@ -7344,7 +7344,7 @@
     </row>
     <row r="188" spans="1:10">
       <c r="A188">
-        <v>1667930400</v>
+        <v>1667919600</v>
       </c>
       <c r="B188" t="s">
         <v>196</v>
@@ -7376,7 +7376,7 @@
     </row>
     <row r="189" spans="1:10">
       <c r="A189">
-        <v>1667934000</v>
+        <v>1667923200</v>
       </c>
       <c r="B189" t="s">
         <v>197</v>
@@ -7408,7 +7408,7 @@
     </row>
     <row r="190" spans="1:10">
       <c r="A190">
-        <v>1667937600</v>
+        <v>1667926800</v>
       </c>
       <c r="B190" t="s">
         <v>198</v>
@@ -7440,7 +7440,7 @@
     </row>
     <row r="191" spans="1:10">
       <c r="A191">
-        <v>1667941200</v>
+        <v>1667930400</v>
       </c>
       <c r="B191" t="s">
         <v>199</v>
@@ -7472,7 +7472,7 @@
     </row>
     <row r="192" spans="1:10">
       <c r="A192">
-        <v>1667944800</v>
+        <v>1667934000</v>
       </c>
       <c r="B192" t="s">
         <v>200</v>
@@ -7504,7 +7504,7 @@
     </row>
     <row r="193" spans="1:10">
       <c r="A193">
-        <v>1667948400</v>
+        <v>1667937600</v>
       </c>
       <c r="B193" t="s">
         <v>201</v>
@@ -7536,7 +7536,7 @@
     </row>
     <row r="194" spans="1:10">
       <c r="A194">
-        <v>1667952000</v>
+        <v>1667941200</v>
       </c>
       <c r="B194" t="s">
         <v>202</v>
@@ -7568,7 +7568,7 @@
     </row>
     <row r="195" spans="1:10">
       <c r="A195">
-        <v>1667955600</v>
+        <v>1667944800</v>
       </c>
       <c r="B195" t="s">
         <v>203</v>
@@ -7600,7 +7600,7 @@
     </row>
     <row r="196" spans="1:10">
       <c r="A196">
-        <v>1667959200</v>
+        <v>1667948400</v>
       </c>
       <c r="B196" t="s">
         <v>204</v>
@@ -7632,7 +7632,7 @@
     </row>
     <row r="197" spans="1:10">
       <c r="A197">
-        <v>1667962800</v>
+        <v>1667952000</v>
       </c>
       <c r="B197" t="s">
         <v>205</v>
@@ -7664,7 +7664,7 @@
     </row>
     <row r="198" spans="1:10">
       <c r="A198">
-        <v>1667966400</v>
+        <v>1667955600</v>
       </c>
       <c r="B198" t="s">
         <v>206</v>
@@ -7696,7 +7696,7 @@
     </row>
     <row r="199" spans="1:10">
       <c r="A199">
-        <v>1667970000</v>
+        <v>1667959200</v>
       </c>
       <c r="B199" t="s">
         <v>207</v>
@@ -7728,7 +7728,7 @@
     </row>
     <row r="200" spans="1:10">
       <c r="A200">
-        <v>1667973600</v>
+        <v>1667962800</v>
       </c>
       <c r="B200" t="s">
         <v>208</v>
@@ -7760,7 +7760,7 @@
     </row>
     <row r="201" spans="1:10">
       <c r="A201">
-        <v>1667977200</v>
+        <v>1667966400</v>
       </c>
       <c r="B201" t="s">
         <v>209</v>
@@ -7792,7 +7792,7 @@
     </row>
     <row r="202" spans="1:10">
       <c r="A202">
-        <v>1667980800</v>
+        <v>1667970000</v>
       </c>
       <c r="B202" t="s">
         <v>210</v>
@@ -7824,7 +7824,7 @@
     </row>
     <row r="203" spans="1:10">
       <c r="A203">
-        <v>1667984400</v>
+        <v>1667973600</v>
       </c>
       <c r="B203" t="s">
         <v>211</v>
@@ -7856,7 +7856,7 @@
     </row>
     <row r="204" spans="1:10">
       <c r="A204">
-        <v>1667988000</v>
+        <v>1667977200</v>
       </c>
       <c r="B204" t="s">
         <v>212</v>
@@ -7888,7 +7888,7 @@
     </row>
     <row r="205" spans="1:10">
       <c r="A205">
-        <v>1667991600</v>
+        <v>1667980800</v>
       </c>
       <c r="B205" t="s">
         <v>213</v>
@@ -7920,7 +7920,7 @@
     </row>
     <row r="206" spans="1:10">
       <c r="A206">
-        <v>1667995200</v>
+        <v>1667984400</v>
       </c>
       <c r="B206" t="s">
         <v>214</v>
@@ -7952,7 +7952,7 @@
     </row>
     <row r="207" spans="1:10">
       <c r="A207">
-        <v>1667998800</v>
+        <v>1667988000</v>
       </c>
       <c r="B207" t="s">
         <v>215</v>
@@ -7984,7 +7984,7 @@
     </row>
     <row r="208" spans="1:10">
       <c r="A208">
-        <v>1668002400</v>
+        <v>1667991600</v>
       </c>
       <c r="B208" t="s">
         <v>216</v>
@@ -8016,7 +8016,7 @@
     </row>
     <row r="209" spans="1:10">
       <c r="A209">
-        <v>1668006000</v>
+        <v>1667995200</v>
       </c>
       <c r="B209" t="s">
         <v>217</v>
@@ -8048,7 +8048,7 @@
     </row>
     <row r="210" spans="1:10">
       <c r="A210">
-        <v>1668009600</v>
+        <v>1667998800</v>
       </c>
       <c r="B210" t="s">
         <v>218</v>
@@ -8080,7 +8080,7 @@
     </row>
     <row r="211" spans="1:10">
       <c r="A211">
-        <v>1668013200</v>
+        <v>1668002400</v>
       </c>
       <c r="B211" t="s">
         <v>219</v>
@@ -8112,7 +8112,7 @@
     </row>
     <row r="212" spans="1:10">
       <c r="A212">
-        <v>1668016800</v>
+        <v>1668006000</v>
       </c>
       <c r="B212" t="s">
         <v>220</v>
@@ -8144,7 +8144,7 @@
     </row>
     <row r="213" spans="1:10">
       <c r="A213">
-        <v>1668020400</v>
+        <v>1668009600</v>
       </c>
       <c r="B213" t="s">
         <v>221</v>
@@ -8176,7 +8176,7 @@
     </row>
     <row r="214" spans="1:10">
       <c r="A214">
-        <v>1668024000</v>
+        <v>1668013200</v>
       </c>
       <c r="B214" t="s">
         <v>222</v>
@@ -8208,7 +8208,7 @@
     </row>
     <row r="215" spans="1:10">
       <c r="A215">
-        <v>1668027600</v>
+        <v>1668016800</v>
       </c>
       <c r="B215" t="s">
         <v>223</v>
@@ -8240,7 +8240,7 @@
     </row>
     <row r="216" spans="1:10">
       <c r="A216">
-        <v>1668031200</v>
+        <v>1668020400</v>
       </c>
       <c r="B216" t="s">
         <v>224</v>
@@ -8272,7 +8272,7 @@
     </row>
     <row r="217" spans="1:10">
       <c r="A217">
-        <v>1668034800</v>
+        <v>1668024000</v>
       </c>
       <c r="B217" t="s">
         <v>225</v>
@@ -8304,7 +8304,7 @@
     </row>
     <row r="218" spans="1:10">
       <c r="A218">
-        <v>1668038400</v>
+        <v>1668027600</v>
       </c>
       <c r="B218" t="s">
         <v>226</v>
@@ -8336,7 +8336,7 @@
     </row>
     <row r="219" spans="1:10">
       <c r="A219">
-        <v>1668042000</v>
+        <v>1668031200</v>
       </c>
       <c r="B219" t="s">
         <v>227</v>
@@ -8368,7 +8368,7 @@
     </row>
     <row r="220" spans="1:10">
       <c r="A220">
-        <v>1668045600</v>
+        <v>1668034800</v>
       </c>
       <c r="B220" t="s">
         <v>228</v>
@@ -8400,7 +8400,7 @@
     </row>
     <row r="221" spans="1:10">
       <c r="A221">
-        <v>1668049200</v>
+        <v>1668038400</v>
       </c>
       <c r="B221" t="s">
         <v>229</v>
@@ -8432,7 +8432,7 @@
     </row>
     <row r="222" spans="1:10">
       <c r="A222">
-        <v>1668052800</v>
+        <v>1668042000</v>
       </c>
       <c r="B222" t="s">
         <v>230</v>
@@ -8464,7 +8464,7 @@
     </row>
     <row r="223" spans="1:10">
       <c r="A223">
-        <v>1668056400</v>
+        <v>1668045600</v>
       </c>
       <c r="B223" t="s">
         <v>231</v>
@@ -8496,7 +8496,7 @@
     </row>
     <row r="224" spans="1:10">
       <c r="A224">
-        <v>1668060000</v>
+        <v>1668049200</v>
       </c>
       <c r="B224" t="s">
         <v>232</v>
@@ -8528,7 +8528,7 @@
     </row>
     <row r="225" spans="1:10">
       <c r="A225">
-        <v>1668063600</v>
+        <v>1668052800</v>
       </c>
       <c r="B225" t="s">
         <v>233</v>
@@ -8560,7 +8560,7 @@
     </row>
     <row r="226" spans="1:10">
       <c r="A226">
-        <v>1668067200</v>
+        <v>1668056400</v>
       </c>
       <c r="B226" t="s">
         <v>234</v>
@@ -8592,7 +8592,7 @@
     </row>
     <row r="227" spans="1:10">
       <c r="A227">
-        <v>1668070800</v>
+        <v>1668060000</v>
       </c>
       <c r="B227" t="s">
         <v>235</v>
@@ -8624,7 +8624,7 @@
     </row>
     <row r="228" spans="1:10">
       <c r="A228">
-        <v>1668074400</v>
+        <v>1668063600</v>
       </c>
       <c r="B228" t="s">
         <v>236</v>
@@ -8656,7 +8656,7 @@
     </row>
     <row r="229" spans="1:10">
       <c r="A229">
-        <v>1668078000</v>
+        <v>1668067200</v>
       </c>
       <c r="B229" t="s">
         <v>237</v>
@@ -8688,7 +8688,7 @@
     </row>
     <row r="230" spans="1:10">
       <c r="A230">
-        <v>1668081600</v>
+        <v>1668070800</v>
       </c>
       <c r="B230" t="s">
         <v>238</v>
@@ -8720,7 +8720,7 @@
     </row>
     <row r="231" spans="1:10">
       <c r="A231">
-        <v>1668085200</v>
+        <v>1668074400</v>
       </c>
       <c r="B231" t="s">
         <v>239</v>
@@ -8752,7 +8752,7 @@
     </row>
     <row r="232" spans="1:10">
       <c r="A232">
-        <v>1668088800</v>
+        <v>1668078000</v>
       </c>
       <c r="B232" t="s">
         <v>240</v>
@@ -8784,7 +8784,7 @@
     </row>
     <row r="233" spans="1:10">
       <c r="A233">
-        <v>1668092400</v>
+        <v>1668081600</v>
       </c>
       <c r="B233" t="s">
         <v>241</v>
@@ -8816,7 +8816,7 @@
     </row>
     <row r="234" spans="1:10">
       <c r="A234">
-        <v>1668096000</v>
+        <v>1668085200</v>
       </c>
       <c r="B234" t="s">
         <v>242</v>
@@ -8848,7 +8848,7 @@
     </row>
     <row r="235" spans="1:10">
       <c r="A235">
-        <v>1668099600</v>
+        <v>1668088800</v>
       </c>
       <c r="B235" t="s">
         <v>243</v>
@@ -8880,7 +8880,7 @@
     </row>
     <row r="236" spans="1:10">
       <c r="A236">
-        <v>1668103200</v>
+        <v>1668092400</v>
       </c>
       <c r="B236" t="s">
         <v>244</v>
@@ -8912,7 +8912,7 @@
     </row>
     <row r="237" spans="1:10">
       <c r="A237">
-        <v>1668106800</v>
+        <v>1668096000</v>
       </c>
       <c r="B237" t="s">
         <v>245</v>
@@ -8944,7 +8944,7 @@
     </row>
     <row r="238" spans="1:10">
       <c r="A238">
-        <v>1668110400</v>
+        <v>1668099600</v>
       </c>
       <c r="B238" t="s">
         <v>246</v>
@@ -8976,7 +8976,7 @@
     </row>
     <row r="239" spans="1:10">
       <c r="A239">
-        <v>1668114000</v>
+        <v>1668103200</v>
       </c>
       <c r="B239" t="s">
         <v>247</v>
@@ -9008,7 +9008,7 @@
     </row>
     <row r="240" spans="1:10">
       <c r="A240">
-        <v>1668117600</v>
+        <v>1668106800</v>
       </c>
       <c r="B240" t="s">
         <v>248</v>
@@ -9040,7 +9040,7 @@
     </row>
     <row r="241" spans="1:10">
       <c r="A241">
-        <v>1668121200</v>
+        <v>1668110400</v>
       </c>
       <c r="B241" t="s">
         <v>249</v>
@@ -9072,7 +9072,7 @@
     </row>
     <row r="242" spans="1:10">
       <c r="A242">
-        <v>1668124800</v>
+        <v>1668114000</v>
       </c>
       <c r="B242" t="s">
         <v>250</v>
@@ -9104,7 +9104,7 @@
     </row>
     <row r="243" spans="1:10">
       <c r="A243">
-        <v>1668128400</v>
+        <v>1668117600</v>
       </c>
       <c r="B243" t="s">
         <v>251</v>
@@ -9136,7 +9136,7 @@
     </row>
     <row r="244" spans="1:10">
       <c r="A244">
-        <v>1668132000</v>
+        <v>1668121200</v>
       </c>
       <c r="B244" t="s">
         <v>252</v>
@@ -9168,7 +9168,7 @@
     </row>
     <row r="245" spans="1:10">
       <c r="A245">
-        <v>1668135600</v>
+        <v>1668124800</v>
       </c>
       <c r="B245" t="s">
         <v>253</v>
@@ -9200,7 +9200,7 @@
     </row>
     <row r="246" spans="1:10">
       <c r="A246">
-        <v>1668139200</v>
+        <v>1668128400</v>
       </c>
       <c r="B246" t="s">
         <v>254</v>
@@ -9232,7 +9232,7 @@
     </row>
     <row r="247" spans="1:10">
       <c r="A247">
-        <v>1668142800</v>
+        <v>1668132000</v>
       </c>
       <c r="B247" t="s">
         <v>255</v>
@@ -9264,7 +9264,7 @@
     </row>
     <row r="248" spans="1:10">
       <c r="A248">
-        <v>1668146400</v>
+        <v>1668135600</v>
       </c>
       <c r="B248" t="s">
         <v>256</v>
@@ -9296,7 +9296,7 @@
     </row>
     <row r="249" spans="1:10">
       <c r="A249">
-        <v>1668150000</v>
+        <v>1668139200</v>
       </c>
       <c r="B249" t="s">
         <v>257</v>
@@ -9328,7 +9328,7 @@
     </row>
     <row r="250" spans="1:10">
       <c r="A250">
-        <v>1668153600</v>
+        <v>1668142800</v>
       </c>
       <c r="B250" t="s">
         <v>258</v>
@@ -9360,7 +9360,7 @@
     </row>
     <row r="251" spans="1:10">
       <c r="A251">
-        <v>1668157200</v>
+        <v>1668146400</v>
       </c>
       <c r="B251" t="s">
         <v>259</v>
@@ -9392,7 +9392,7 @@
     </row>
     <row r="252" spans="1:10">
       <c r="A252">
-        <v>1668160800</v>
+        <v>1668150000</v>
       </c>
       <c r="B252" t="s">
         <v>260</v>
@@ -9424,7 +9424,7 @@
     </row>
     <row r="253" spans="1:10">
       <c r="A253">
-        <v>1668164400</v>
+        <v>1668153600</v>
       </c>
       <c r="B253" t="s">
         <v>261</v>
@@ -9456,7 +9456,7 @@
     </row>
     <row r="254" spans="1:10">
       <c r="A254">
-        <v>1668168000</v>
+        <v>1668157200</v>
       </c>
       <c r="B254" t="s">
         <v>262</v>
@@ -9488,7 +9488,7 @@
     </row>
     <row r="255" spans="1:10">
       <c r="A255">
-        <v>1668171600</v>
+        <v>1668160800</v>
       </c>
       <c r="B255" t="s">
         <v>263</v>
@@ -9520,7 +9520,7 @@
     </row>
     <row r="256" spans="1:10">
       <c r="A256">
-        <v>1668175200</v>
+        <v>1668164400</v>
       </c>
       <c r="B256" t="s">
         <v>264</v>
@@ -9552,7 +9552,7 @@
     </row>
     <row r="257" spans="1:10">
       <c r="A257">
-        <v>1668178800</v>
+        <v>1668168000</v>
       </c>
       <c r="B257" t="s">
         <v>265</v>
@@ -9584,7 +9584,7 @@
     </row>
     <row r="258" spans="1:10">
       <c r="A258">
-        <v>1668182400</v>
+        <v>1668171600</v>
       </c>
       <c r="B258" t="s">
         <v>266</v>
@@ -9616,7 +9616,7 @@
     </row>
     <row r="259" spans="1:10">
       <c r="A259">
-        <v>1668186000</v>
+        <v>1668175200</v>
       </c>
       <c r="B259" t="s">
         <v>267</v>
@@ -9648,7 +9648,7 @@
     </row>
     <row r="260" spans="1:10">
       <c r="A260">
-        <v>1668189600</v>
+        <v>1668178800</v>
       </c>
       <c r="B260" t="s">
         <v>268</v>
@@ -9680,7 +9680,7 @@
     </row>
     <row r="261" spans="1:10">
       <c r="A261">
-        <v>1668193200</v>
+        <v>1668182400</v>
       </c>
       <c r="B261" t="s">
         <v>269</v>
@@ -9712,7 +9712,7 @@
     </row>
     <row r="262" spans="1:10">
       <c r="A262">
-        <v>1668196800</v>
+        <v>1668186000</v>
       </c>
       <c r="B262" t="s">
         <v>270</v>
@@ -9744,7 +9744,7 @@
     </row>
     <row r="263" spans="1:10">
       <c r="A263">
-        <v>1668200400</v>
+        <v>1668189600</v>
       </c>
       <c r="B263" t="s">
         <v>271</v>
@@ -9776,7 +9776,7 @@
     </row>
     <row r="264" spans="1:10">
       <c r="A264">
-        <v>1668204000</v>
+        <v>1668193200</v>
       </c>
       <c r="B264" t="s">
         <v>272</v>
@@ -9808,7 +9808,7 @@
     </row>
     <row r="265" spans="1:10">
       <c r="A265">
-        <v>1668207600</v>
+        <v>1668196800</v>
       </c>
       <c r="B265" t="s">
         <v>273</v>
@@ -9840,7 +9840,7 @@
     </row>
     <row r="266" spans="1:10">
       <c r="A266">
-        <v>1668211200</v>
+        <v>1668200400</v>
       </c>
       <c r="B266" t="s">
         <v>274</v>
@@ -9872,7 +9872,7 @@
     </row>
     <row r="267" spans="1:10">
       <c r="A267">
-        <v>1668214800</v>
+        <v>1668204000</v>
       </c>
       <c r="B267" t="s">
         <v>275</v>
@@ -9904,7 +9904,7 @@
     </row>
     <row r="268" spans="1:10">
       <c r="A268">
-        <v>1668218400</v>
+        <v>1668207600</v>
       </c>
       <c r="B268" t="s">
         <v>276</v>
@@ -9936,7 +9936,7 @@
     </row>
     <row r="269" spans="1:10">
       <c r="A269">
-        <v>1668222000</v>
+        <v>1668211200</v>
       </c>
       <c r="B269" t="s">
         <v>277</v>
@@ -9968,7 +9968,7 @@
     </row>
     <row r="270" spans="1:10">
       <c r="A270">
-        <v>1668225600</v>
+        <v>1668214800</v>
       </c>
       <c r="B270" t="s">
         <v>278</v>
@@ -10000,7 +10000,7 @@
     </row>
     <row r="271" spans="1:10">
       <c r="A271">
-        <v>1668229200</v>
+        <v>1668218400</v>
       </c>
       <c r="B271" t="s">
         <v>279</v>
@@ -10032,7 +10032,7 @@
     </row>
     <row r="272" spans="1:10">
       <c r="A272">
-        <v>1668232800</v>
+        <v>1668222000</v>
       </c>
       <c r="B272" t="s">
         <v>280</v>
@@ -10064,7 +10064,7 @@
     </row>
     <row r="273" spans="1:10">
       <c r="A273">
-        <v>1668236400</v>
+        <v>1668225600</v>
       </c>
       <c r="B273" t="s">
         <v>281</v>
@@ -10096,7 +10096,7 @@
     </row>
     <row r="274" spans="1:10">
       <c r="A274">
-        <v>1668240000</v>
+        <v>1668229200</v>
       </c>
       <c r="B274" t="s">
         <v>282</v>
@@ -10128,7 +10128,7 @@
     </row>
     <row r="275" spans="1:10">
       <c r="A275">
-        <v>1668243600</v>
+        <v>1668232800</v>
       </c>
       <c r="B275" t="s">
         <v>283</v>
@@ -10160,7 +10160,7 @@
     </row>
     <row r="276" spans="1:10">
       <c r="A276">
-        <v>1668247200</v>
+        <v>1668236400</v>
       </c>
       <c r="B276" t="s">
         <v>284</v>
@@ -10192,7 +10192,7 @@
     </row>
     <row r="277" spans="1:10">
       <c r="A277">
-        <v>1668250800</v>
+        <v>1668240000</v>
       </c>
       <c r="B277" t="s">
         <v>285</v>
@@ -10224,7 +10224,7 @@
     </row>
     <row r="278" spans="1:10">
       <c r="A278">
-        <v>1668254400</v>
+        <v>1668243600</v>
       </c>
       <c r="B278" t="s">
         <v>286</v>
@@ -10256,7 +10256,7 @@
     </row>
     <row r="279" spans="1:10">
       <c r="A279">
-        <v>1668258000</v>
+        <v>1668247200</v>
       </c>
       <c r="B279" t="s">
         <v>287</v>
@@ -10288,7 +10288,7 @@
     </row>
     <row r="280" spans="1:10">
       <c r="A280">
-        <v>1668261600</v>
+        <v>1668250800</v>
       </c>
       <c r="B280" t="s">
         <v>288</v>
@@ -10320,7 +10320,7 @@
     </row>
     <row r="281" spans="1:10">
       <c r="A281">
-        <v>1668265200</v>
+        <v>1668254400</v>
       </c>
       <c r="B281" t="s">
         <v>289</v>
@@ -10352,7 +10352,7 @@
     </row>
     <row r="282" spans="1:10">
       <c r="A282">
-        <v>1668268800</v>
+        <v>1668258000</v>
       </c>
       <c r="B282" t="s">
         <v>290</v>
@@ -10384,7 +10384,7 @@
     </row>
     <row r="283" spans="1:10">
       <c r="A283">
-        <v>1668272400</v>
+        <v>1668261600</v>
       </c>
       <c r="B283" t="s">
         <v>291</v>
@@ -10416,7 +10416,7 @@
     </row>
     <row r="284" spans="1:10">
       <c r="A284">
-        <v>1668276000</v>
+        <v>1668265200</v>
       </c>
       <c r="B284" t="s">
         <v>292</v>
@@ -10448,7 +10448,7 @@
     </row>
     <row r="285" spans="1:10">
       <c r="A285">
-        <v>1668279600</v>
+        <v>1668268800</v>
       </c>
       <c r="B285" t="s">
         <v>293</v>
@@ -10480,7 +10480,7 @@
     </row>
     <row r="286" spans="1:10">
       <c r="A286">
-        <v>1668283200</v>
+        <v>1668272400</v>
       </c>
       <c r="B286" t="s">
         <v>294</v>
@@ -10512,7 +10512,7 @@
     </row>
     <row r="287" spans="1:10">
       <c r="A287">
-        <v>1668286800</v>
+        <v>1668276000</v>
       </c>
       <c r="B287" t="s">
         <v>295</v>
@@ -10544,7 +10544,7 @@
     </row>
     <row r="288" spans="1:10">
       <c r="A288">
-        <v>1668290400</v>
+        <v>1668279600</v>
       </c>
       <c r="B288" t="s">
         <v>296</v>
@@ -10576,7 +10576,7 @@
     </row>
     <row r="289" spans="1:10">
       <c r="A289">
-        <v>1668294000</v>
+        <v>1668283200</v>
       </c>
       <c r="B289" t="s">
         <v>297</v>
@@ -10608,7 +10608,7 @@
     </row>
     <row r="290" spans="1:10">
       <c r="A290">
-        <v>1668297600</v>
+        <v>1668286800</v>
       </c>
       <c r="B290" t="s">
         <v>298</v>
@@ -10640,7 +10640,7 @@
     </row>
     <row r="291" spans="1:10">
       <c r="A291">
-        <v>1668301200</v>
+        <v>1668290400</v>
       </c>
       <c r="B291" t="s">
         <v>299</v>
@@ -10672,7 +10672,7 @@
     </row>
     <row r="292" spans="1:10">
       <c r="A292">
-        <v>1668304800</v>
+        <v>1668294000</v>
       </c>
       <c r="B292" t="s">
         <v>300</v>
@@ -10704,7 +10704,7 @@
     </row>
     <row r="293" spans="1:10">
       <c r="A293">
-        <v>1668308400</v>
+        <v>1668297600</v>
       </c>
       <c r="B293" t="s">
         <v>301</v>
@@ -10736,7 +10736,7 @@
     </row>
     <row r="294" spans="1:10">
       <c r="A294">
-        <v>1668312000</v>
+        <v>1668301200</v>
       </c>
       <c r="B294" t="s">
         <v>302</v>
@@ -10768,7 +10768,7 @@
     </row>
     <row r="295" spans="1:10">
       <c r="A295">
-        <v>1668315600</v>
+        <v>1668304800</v>
       </c>
       <c r="B295" t="s">
         <v>303</v>
@@ -10800,7 +10800,7 @@
     </row>
     <row r="296" spans="1:10">
       <c r="A296">
-        <v>1668319200</v>
+        <v>1668308400</v>
       </c>
       <c r="B296" t="s">
         <v>304</v>
@@ -10832,7 +10832,7 @@
     </row>
     <row r="297" spans="1:10">
       <c r="A297">
-        <v>1668322800</v>
+        <v>1668312000</v>
       </c>
       <c r="B297" t="s">
         <v>305</v>
@@ -10864,7 +10864,7 @@
     </row>
     <row r="298" spans="1:10">
       <c r="A298">
-        <v>1668326400</v>
+        <v>1668315600</v>
       </c>
       <c r="B298" t="s">
         <v>306</v>
@@ -10896,7 +10896,7 @@
     </row>
     <row r="299" spans="1:10">
       <c r="A299">
-        <v>1668330000</v>
+        <v>1668319200</v>
       </c>
       <c r="B299" t="s">
         <v>307</v>
@@ -10928,7 +10928,7 @@
     </row>
     <row r="300" spans="1:10">
       <c r="A300">
-        <v>1668333600</v>
+        <v>1668322800</v>
       </c>
       <c r="B300" t="s">
         <v>308</v>
@@ -10960,7 +10960,7 @@
     </row>
     <row r="301" spans="1:10">
       <c r="A301">
-        <v>1668337200</v>
+        <v>1668326400</v>
       </c>
       <c r="B301" t="s">
         <v>309</v>
@@ -10992,7 +10992,7 @@
     </row>
     <row r="302" spans="1:10">
       <c r="A302">
-        <v>1668340800</v>
+        <v>1668330000</v>
       </c>
       <c r="B302" t="s">
         <v>310</v>
@@ -11024,7 +11024,7 @@
     </row>
     <row r="303" spans="1:10">
       <c r="A303">
-        <v>1668344400</v>
+        <v>1668333600</v>
       </c>
       <c r="B303" t="s">
         <v>311</v>
@@ -11056,7 +11056,7 @@
     </row>
     <row r="304" spans="1:10">
       <c r="A304">
-        <v>1668348000</v>
+        <v>1668337200</v>
       </c>
       <c r="B304" t="s">
         <v>312</v>
@@ -11088,7 +11088,7 @@
     </row>
     <row r="305" spans="1:10">
       <c r="A305">
-        <v>1668351600</v>
+        <v>1668340800</v>
       </c>
       <c r="B305" t="s">
         <v>313</v>
@@ -11120,7 +11120,7 @@
     </row>
     <row r="306" spans="1:10">
       <c r="A306">
-        <v>1668355200</v>
+        <v>1668344400</v>
       </c>
       <c r="B306" t="s">
         <v>314</v>
@@ -11152,7 +11152,7 @@
     </row>
     <row r="307" spans="1:10">
       <c r="A307">
-        <v>1668358800</v>
+        <v>1668348000</v>
       </c>
       <c r="B307" t="s">
         <v>315</v>
@@ -11184,7 +11184,7 @@
     </row>
     <row r="308" spans="1:10">
       <c r="A308">
-        <v>1668362400</v>
+        <v>1668351600</v>
       </c>
       <c r="B308" t="s">
         <v>316</v>
@@ -11216,7 +11216,7 @@
     </row>
     <row r="309" spans="1:10">
       <c r="A309">
-        <v>1668196800</v>
+        <v>1668186000</v>
       </c>
       <c r="B309" t="s">
         <v>270</v>
@@ -11245,7 +11245,7 @@
     </row>
     <row r="310" spans="1:10">
       <c r="A310">
-        <v>1668200400</v>
+        <v>1668189600</v>
       </c>
       <c r="B310" t="s">
         <v>271</v>
@@ -11274,7 +11274,7 @@
     </row>
     <row r="311" spans="1:10">
       <c r="A311">
-        <v>1668204000</v>
+        <v>1668193200</v>
       </c>
       <c r="B311" t="s">
         <v>272</v>
@@ -11303,7 +11303,7 @@
     </row>
     <row r="312" spans="1:10">
       <c r="A312">
-        <v>1668207600</v>
+        <v>1668196800</v>
       </c>
       <c r="B312" t="s">
         <v>273</v>
@@ -11332,7 +11332,7 @@
     </row>
     <row r="313" spans="1:10">
       <c r="A313">
-        <v>1668211200</v>
+        <v>1668200400</v>
       </c>
       <c r="B313" t="s">
         <v>274</v>
@@ -11361,7 +11361,7 @@
     </row>
     <row r="314" spans="1:10">
       <c r="A314">
-        <v>1668214800</v>
+        <v>1668204000</v>
       </c>
       <c r="B314" t="s">
         <v>275</v>
@@ -11390,7 +11390,7 @@
     </row>
     <row r="315" spans="1:10">
       <c r="A315">
-        <v>1668218400</v>
+        <v>1668207600</v>
       </c>
       <c r="B315" t="s">
         <v>276</v>
@@ -11419,7 +11419,7 @@
     </row>
     <row r="316" spans="1:10">
       <c r="A316">
-        <v>1668222000</v>
+        <v>1668211200</v>
       </c>
       <c r="B316" t="s">
         <v>277</v>
@@ -11448,7 +11448,7 @@
     </row>
     <row r="317" spans="1:10">
       <c r="A317">
-        <v>1668225600</v>
+        <v>1668214800</v>
       </c>
       <c r="B317" t="s">
         <v>278</v>
@@ -11477,7 +11477,7 @@
     </row>
     <row r="318" spans="1:10">
       <c r="A318">
-        <v>1668229200</v>
+        <v>1668218400</v>
       </c>
       <c r="B318" t="s">
         <v>279</v>
@@ -11506,7 +11506,7 @@
     </row>
     <row r="319" spans="1:10">
       <c r="A319">
-        <v>1668232800</v>
+        <v>1668222000</v>
       </c>
       <c r="B319" t="s">
         <v>280</v>
@@ -11535,7 +11535,7 @@
     </row>
     <row r="320" spans="1:10">
       <c r="A320">
-        <v>1668236400</v>
+        <v>1668225600</v>
       </c>
       <c r="B320" t="s">
         <v>281</v>
@@ -11564,7 +11564,7 @@
     </row>
     <row r="321" spans="1:10">
       <c r="A321">
-        <v>1668240000</v>
+        <v>1668229200</v>
       </c>
       <c r="B321" t="s">
         <v>282</v>
@@ -11593,7 +11593,7 @@
     </row>
     <row r="322" spans="1:10">
       <c r="A322">
-        <v>1668243600</v>
+        <v>1668232800</v>
       </c>
       <c r="B322" t="s">
         <v>283</v>
@@ -11622,7 +11622,7 @@
     </row>
     <row r="323" spans="1:10">
       <c r="A323">
-        <v>1668247200</v>
+        <v>1668236400</v>
       </c>
       <c r="B323" t="s">
         <v>284</v>
@@ -11651,7 +11651,7 @@
     </row>
     <row r="324" spans="1:10">
       <c r="A324">
-        <v>1668250800</v>
+        <v>1668240000</v>
       </c>
       <c r="B324" t="s">
         <v>285</v>
@@ -11680,7 +11680,7 @@
     </row>
     <row r="325" spans="1:10">
       <c r="A325">
-        <v>1668254400</v>
+        <v>1668243600</v>
       </c>
       <c r="B325" t="s">
         <v>286</v>
@@ -11709,7 +11709,7 @@
     </row>
     <row r="326" spans="1:10">
       <c r="A326">
-        <v>1668258000</v>
+        <v>1668247200</v>
       </c>
       <c r="B326" t="s">
         <v>287</v>
@@ -11738,7 +11738,7 @@
     </row>
     <row r="327" spans="1:10">
       <c r="A327">
-        <v>1668261600</v>
+        <v>1668250800</v>
       </c>
       <c r="B327" t="s">
         <v>288</v>
@@ -11767,7 +11767,7 @@
     </row>
     <row r="328" spans="1:10">
       <c r="A328">
-        <v>1668265200</v>
+        <v>1668254400</v>
       </c>
       <c r="B328" t="s">
         <v>289</v>
@@ -11796,7 +11796,7 @@
     </row>
     <row r="329" spans="1:10">
       <c r="A329">
-        <v>1668268800</v>
+        <v>1668258000</v>
       </c>
       <c r="B329" t="s">
         <v>290</v>
@@ -11825,7 +11825,7 @@
     </row>
     <row r="330" spans="1:10">
       <c r="A330">
-        <v>1668272400</v>
+        <v>1668261600</v>
       </c>
       <c r="B330" t="s">
         <v>291</v>
@@ -11854,7 +11854,7 @@
     </row>
     <row r="331" spans="1:10">
       <c r="A331">
-        <v>1668276000</v>
+        <v>1668265200</v>
       </c>
       <c r="B331" t="s">
         <v>292</v>
@@ -11883,7 +11883,7 @@
     </row>
     <row r="332" spans="1:10">
       <c r="A332">
-        <v>1668279600</v>
+        <v>1668268800</v>
       </c>
       <c r="B332" t="s">
         <v>293</v>
@@ -11912,7 +11912,7 @@
     </row>
     <row r="333" spans="1:10">
       <c r="A333">
-        <v>1668283200</v>
+        <v>1668272400</v>
       </c>
       <c r="B333" t="s">
         <v>294</v>
@@ -11941,7 +11941,7 @@
     </row>
     <row r="334" spans="1:10">
       <c r="A334">
-        <v>1668286800</v>
+        <v>1668276000</v>
       </c>
       <c r="B334" t="s">
         <v>295</v>
@@ -11970,7 +11970,7 @@
     </row>
     <row r="335" spans="1:10">
       <c r="A335">
-        <v>1668290400</v>
+        <v>1668279600</v>
       </c>
       <c r="B335" t="s">
         <v>296</v>
@@ -11999,7 +11999,7 @@
     </row>
     <row r="336" spans="1:10">
       <c r="A336">
-        <v>1668294000</v>
+        <v>1668283200</v>
       </c>
       <c r="B336" t="s">
         <v>297</v>
@@ -12028,7 +12028,7 @@
     </row>
     <row r="337" spans="1:10">
       <c r="A337">
-        <v>1668297600</v>
+        <v>1668286800</v>
       </c>
       <c r="B337" t="s">
         <v>298</v>
@@ -12057,7 +12057,7 @@
     </row>
     <row r="338" spans="1:10">
       <c r="A338">
-        <v>1668301200</v>
+        <v>1668290400</v>
       </c>
       <c r="B338" t="s">
         <v>299</v>
@@ -12086,7 +12086,7 @@
     </row>
     <row r="339" spans="1:10">
       <c r="A339">
-        <v>1668304800</v>
+        <v>1668294000</v>
       </c>
       <c r="B339" t="s">
         <v>300</v>
@@ -12115,7 +12115,7 @@
     </row>
     <row r="340" spans="1:10">
       <c r="A340">
-        <v>1668308400</v>
+        <v>1668297600</v>
       </c>
       <c r="B340" t="s">
         <v>301</v>
@@ -12144,7 +12144,7 @@
     </row>
     <row r="341" spans="1:10">
       <c r="A341">
-        <v>1668312000</v>
+        <v>1668301200</v>
       </c>
       <c r="B341" t="s">
         <v>302</v>
@@ -12173,7 +12173,7 @@
     </row>
     <row r="342" spans="1:10">
       <c r="A342">
-        <v>1668315600</v>
+        <v>1668304800</v>
       </c>
       <c r="B342" t="s">
         <v>303</v>
@@ -12202,7 +12202,7 @@
     </row>
     <row r="343" spans="1:10">
       <c r="A343">
-        <v>1668319200</v>
+        <v>1668308400</v>
       </c>
       <c r="B343" t="s">
         <v>304</v>
@@ -12231,7 +12231,7 @@
     </row>
     <row r="344" spans="1:10">
       <c r="A344">
-        <v>1668322800</v>
+        <v>1668312000</v>
       </c>
       <c r="B344" t="s">
         <v>305</v>
@@ -12260,7 +12260,7 @@
     </row>
     <row r="345" spans="1:10">
       <c r="A345">
-        <v>1668326400</v>
+        <v>1668315600</v>
       </c>
       <c r="B345" t="s">
         <v>306</v>
@@ -12289,7 +12289,7 @@
     </row>
     <row r="346" spans="1:10">
       <c r="A346">
-        <v>1668330000</v>
+        <v>1668319200</v>
       </c>
       <c r="B346" t="s">
         <v>307</v>
@@ -12318,7 +12318,7 @@
     </row>
     <row r="347" spans="1:10">
       <c r="A347">
-        <v>1668333600</v>
+        <v>1668322800</v>
       </c>
       <c r="B347" t="s">
         <v>308</v>
@@ -12347,7 +12347,7 @@
     </row>
     <row r="348" spans="1:10">
       <c r="A348">
-        <v>1668337200</v>
+        <v>1668326400</v>
       </c>
       <c r="B348" t="s">
         <v>309</v>
@@ -12376,7 +12376,7 @@
     </row>
     <row r="349" spans="1:10">
       <c r="A349">
-        <v>1668340800</v>
+        <v>1668330000</v>
       </c>
       <c r="B349" t="s">
         <v>310</v>
@@ -12405,7 +12405,7 @@
     </row>
     <row r="350" spans="1:10">
       <c r="A350">
-        <v>1668344400</v>
+        <v>1668333600</v>
       </c>
       <c r="B350" t="s">
         <v>311</v>
@@ -12434,7 +12434,7 @@
     </row>
     <row r="351" spans="1:10">
       <c r="A351">
-        <v>1668348000</v>
+        <v>1668337200</v>
       </c>
       <c r="B351" t="s">
         <v>312</v>
@@ -12463,7 +12463,7 @@
     </row>
     <row r="352" spans="1:10">
       <c r="A352">
-        <v>1668351600</v>
+        <v>1668340800</v>
       </c>
       <c r="B352" t="s">
         <v>313</v>
@@ -12492,7 +12492,7 @@
     </row>
     <row r="353" spans="1:10">
       <c r="A353">
-        <v>1668355200</v>
+        <v>1668344400</v>
       </c>
       <c r="B353" t="s">
         <v>314</v>
@@ -12521,7 +12521,7 @@
     </row>
     <row r="354" spans="1:10">
       <c r="A354">
-        <v>1668358800</v>
+        <v>1668348000</v>
       </c>
       <c r="B354" t="s">
         <v>315</v>
@@ -12550,7 +12550,7 @@
     </row>
     <row r="355" spans="1:10">
       <c r="A355">
-        <v>1668362400</v>
+        <v>1668351600</v>
       </c>
       <c r="B355" t="s">
         <v>316</v>
@@ -12579,7 +12579,7 @@
     </row>
     <row r="356" spans="1:10">
       <c r="A356">
-        <v>1668366000</v>
+        <v>1668355200</v>
       </c>
       <c r="B356" t="s">
         <v>317</v>
@@ -12608,7 +12608,7 @@
     </row>
     <row r="357" spans="1:10">
       <c r="A357">
-        <v>1668369600</v>
+        <v>1668358800</v>
       </c>
       <c r="B357" t="s">
         <v>318</v>
@@ -12637,7 +12637,7 @@
     </row>
     <row r="358" spans="1:10">
       <c r="A358">
-        <v>1668373200</v>
+        <v>1668362400</v>
       </c>
       <c r="B358" t="s">
         <v>319</v>
@@ -12666,7 +12666,7 @@
     </row>
     <row r="359" spans="1:10">
       <c r="A359">
-        <v>1668376800</v>
+        <v>1668366000</v>
       </c>
       <c r="B359" t="s">
         <v>320</v>
@@ -12695,7 +12695,7 @@
     </row>
     <row r="360" spans="1:10">
       <c r="A360">
-        <v>1668380400</v>
+        <v>1668369600</v>
       </c>
       <c r="B360" t="s">
         <v>321</v>
@@ -12724,7 +12724,7 @@
     </row>
     <row r="361" spans="1:10">
       <c r="A361">
-        <v>1668384000</v>
+        <v>1668373200</v>
       </c>
       <c r="B361" t="s">
         <v>322</v>
@@ -12753,7 +12753,7 @@
     </row>
     <row r="362" spans="1:10">
       <c r="A362">
-        <v>1668387600</v>
+        <v>1668376800</v>
       </c>
       <c r="B362" t="s">
         <v>323</v>
@@ -12782,7 +12782,7 @@
     </row>
     <row r="363" spans="1:10">
       <c r="A363">
-        <v>1668391200</v>
+        <v>1668380400</v>
       </c>
       <c r="B363" t="s">
         <v>324</v>
@@ -12811,7 +12811,7 @@
     </row>
     <row r="364" spans="1:10">
       <c r="A364">
-        <v>1668394800</v>
+        <v>1668384000</v>
       </c>
       <c r="B364" t="s">
         <v>325</v>
@@ -12840,7 +12840,7 @@
     </row>
     <row r="365" spans="1:10">
       <c r="A365">
-        <v>1668398400</v>
+        <v>1668387600</v>
       </c>
       <c r="B365" t="s">
         <v>326</v>

</xml_diff>